<commit_message>
more work on Maxwell bib
</commit_message>
<xml_diff>
--- a/data/primary_studies/Maxwell_et_al_2023/intermediate/missing_maxwell_studies.xlsx
+++ b/data/primary_studies/Maxwell_et_al_2023/intermediate/missing_maxwell_studies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/SERC/CCN/repos/CCRCN-Data-Library/data/primary_studies/Maxwell_et_al_2023/intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981BB83F-4DFD-CF48-9F7E-0F15A12FDE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2FCF3A-1757-6E48-B432-B30BA62D33DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="760" windowWidth="11360" windowHeight="16520" xr2:uid="{7C2753EE-174F-184D-A25A-F8CFD15E56BA}"/>
+    <workbookView xWindow="6720" yWindow="760" windowWidth="16920" windowHeight="16520" xr2:uid="{7C2753EE-174F-184D-A25A-F8CFD15E56BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>doi</t>
   </si>
@@ -168,6 +168,30 @@
   </si>
   <si>
     <t>10.5285/b57ef444-54d4-47f9-8cbf-3cfef1182b55</t>
+  </si>
+  <si>
+    <t>Yando_et_al_2016</t>
+  </si>
+  <si>
+    <t>10.1111/1365-2745.12571</t>
+  </si>
+  <si>
+    <t>Gao_et_al_2016</t>
+  </si>
+  <si>
+    <t>10.1016/j.ecoleng.2016.06.088</t>
+  </si>
+  <si>
+    <t>10.1016/j.ecoleng.2017.05.041</t>
+  </si>
+  <si>
+    <t>Liu_et_al_2017</t>
+  </si>
+  <si>
+    <t>Fu_et_al_2021</t>
+  </si>
+  <si>
+    <t>10.1111/gcb.15348</t>
   </si>
 </sst>
 </file>
@@ -527,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D5F35C9-23F2-154C-BDE6-BC73D500A787}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,6 +738,38 @@
         <v>42</v>
       </c>
     </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update Maxwell hook #106
</commit_message>
<xml_diff>
--- a/data/primary_studies/Maxwell_et_al_2023/intermediate/missing_maxwell_studies.xlsx
+++ b/data/primary_studies/Maxwell_et_al_2023/intermediate/missing_maxwell_studies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/SERC/CCN/repos/CCRCN-Data-Library/data/primary_studies/Maxwell_et_al_2023/intermediate/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/SERC/CCN/repos/CCN-Data-Library/data/primary_studies/Maxwell_et_al_2023/intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2FCF3A-1757-6E48-B432-B30BA62D33DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1651C7-0E08-0E4E-BE41-C2C846A501A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6720" yWindow="760" windowWidth="16920" windowHeight="16520" xr2:uid="{7C2753EE-174F-184D-A25A-F8CFD15E56BA}"/>
   </bookViews>
@@ -104,9 +104,6 @@
     <t>10.1007/s10021-021-00660-6</t>
   </si>
   <si>
-    <t>Miller_et_al_2022</t>
-  </si>
-  <si>
     <t>Noguiera_et_al_2022</t>
   </si>
   <si>
@@ -170,9 +167,6 @@
     <t>10.5285/b57ef444-54d4-47f9-8cbf-3cfef1182b55</t>
   </si>
   <si>
-    <t>Yando_et_al_2016</t>
-  </si>
-  <si>
     <t>10.1111/1365-2745.12571</t>
   </si>
   <si>
@@ -192,6 +186,12 @@
   </si>
   <si>
     <t>10.1111/gcb.15348</t>
+  </si>
+  <si>
+    <t>Yando_et_al_2016_marsh</t>
+  </si>
+  <si>
+    <t>Miller_et_al_2022_Scotland</t>
   </si>
 </sst>
 </file>
@@ -255,9 +255,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -295,7 +295,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -401,7 +401,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -543,7 +543,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -554,7 +554,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -652,122 +652,122 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
         <v>40</v>
-      </c>
-      <c r="B21" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>